<commit_message>
* Mejoras en formulario dinamico
</commit_message>
<xml_diff>
--- a/Documentos/transacciones para sistema.xlsx
+++ b/Documentos/transacciones para sistema.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMontilla\source\repos\JuanMontillaTech\HADA\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9672DE3-921B-4D95-8DA8-A802645C608F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -233,9 +244,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -285,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +311,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,11 +393,32 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,31 +428,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Celda de comprobación" xfId="2" builtinId="23"/>
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -692,1636 +713,1643 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D172"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" hidden="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6">
         <f>D5+D6</f>
         <v>17700</v>
       </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" ht="1.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <f>C3</f>
         <v>17700</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
         <f>D6*18%</f>
         <v>2700</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
         <v>15000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21">
         <v>12000</v>
       </c>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22">
         <v>12000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6">
         <f>D16+D17</f>
         <v>15340</v>
       </c>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <f>C14</f>
         <v>15340</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6">
         <f>D17*18%</f>
         <v>2340</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6">
         <v>13000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6">
         <v>9000</v>
       </c>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8">
         <v>9000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="12">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="6"/>
+      <c r="C21" s="9">
         <f>SUM(C14:C19)</f>
         <v>24340</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="9">
         <f>SUM(D14:D19)</f>
         <v>24340</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6">
         <v>3500</v>
       </c>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9">
+      <c r="B28" s="5"/>
+      <c r="C28" s="6">
         <f>C27*18%</f>
         <v>630</v>
       </c>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>A19</f>
         <v>Inventarios de mercancias</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9">
+      <c r="B29" s="5"/>
+      <c r="C29" s="6">
         <v>3000</v>
       </c>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>A3</f>
         <v>Cuentas por cobrar</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6">
         <f>C27+C28</f>
         <v>4130</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>A4</f>
         <v xml:space="preserve">Tecno Advanced Group </v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="5">
         <f>C27+C28</f>
         <v>4130</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>A18</f>
         <v>Costo de ventas</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11">
+      <c r="B32" s="12"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8">
         <f>C29</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="12">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="5"/>
+      <c r="C34" s="9">
         <f>SUM(C27:C33)</f>
         <v>7130</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="9">
         <f>SUM(D27:D33)</f>
         <v>7130</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9">
+      <c r="B40" s="5"/>
+      <c r="C40" s="6">
         <f>D42+D43</f>
         <v>5900</v>
       </c>
-      <c r="D40" s="9"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="5">
         <f>C40</f>
         <v>5900</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>A29</f>
         <v>Inventarios de mercancias</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6">
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="11">
+      <c r="B43" s="5"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="8">
         <f>D42*18%</f>
         <v>900</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="12">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="5"/>
+      <c r="C45" s="9">
         <f>SUM(C40:C44)</f>
         <v>5900</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="9">
         <f>SUM(D40:D44)</f>
         <v>5900</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="5"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="18"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5">
         <f>C14</f>
         <v>15340</v>
       </c>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15">
+      <c r="B51" s="5"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12">
         <f>C50</f>
         <v>15340</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
-      <c r="C53" s="12">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="5"/>
+      <c r="C53" s="9">
         <f>SUM(C50:C52)</f>
         <v>15340</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D53" s="9">
         <f>SUM(D50:D52)</f>
         <v>15340</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="8"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="8"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" s="5"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="5"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="18"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="str">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="str">
         <f>A50</f>
         <v>Banco Reservas</v>
       </c>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8">
+      <c r="B59" s="5"/>
+      <c r="C59" s="5">
         <f>C3</f>
         <v>17700</v>
       </c>
-      <c r="D59" s="8"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
+      <c r="D59" s="5"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5">
         <f>C59</f>
         <v>17700</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f>A4</f>
         <v xml:space="preserve">Tecno Advanced Group </v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="12">
         <f>D60</f>
         <v>17700</v>
       </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="8"/>
-      <c r="C63" s="12">
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B63" s="5"/>
+      <c r="C63" s="9">
         <f>SUM(C59:C62)</f>
         <v>17700</v>
       </c>
-      <c r="D63" s="12">
+      <c r="D63" s="9">
         <f>SUM(D59:D62)</f>
         <v>17700</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="18"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="str">
         <f>A42</f>
         <v>Inventarios de mercancias</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9">
+      <c r="B68" s="5"/>
+      <c r="C68" s="6">
         <v>25000</v>
       </c>
-      <c r="D68" s="9"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>18</v>
       </c>
-      <c r="B69" s="8"/>
-      <c r="C69" s="9">
+      <c r="B69" s="5"/>
+      <c r="C69" s="6">
         <f>C68*18%</f>
         <v>4500</v>
       </c>
-      <c r="D69" s="9"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="str">
         <f>A41</f>
         <v>Zuleica Solutions</v>
       </c>
-      <c r="B70" s="8"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11">
+      <c r="B70" s="5"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8">
         <f>C68+C69</f>
         <v>29500</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="8"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="8"/>
-      <c r="C72" s="12">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="5"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B72" s="5"/>
+      <c r="C72" s="9">
         <f>SUM(C68:C71)</f>
         <v>29500</v>
       </c>
-      <c r="D72" s="12">
+      <c r="D72" s="9">
         <f>SUM(D68:D71)</f>
         <v>29500</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="18"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>24</v>
       </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8">
+      <c r="B76" s="5"/>
+      <c r="C76" s="5">
         <v>10000</v>
       </c>
-      <c r="D76" s="8"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>25</v>
       </c>
-      <c r="B77" s="8">
+      <c r="B77" s="5">
         <v>10000</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>26</v>
       </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5">
         <v>10000</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="18"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>28</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5">
         <v>20000</v>
       </c>
-      <c r="D82" s="8"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>29</v>
       </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8">
+      <c r="B83" s="5"/>
+      <c r="C83" s="5">
         <v>3600</v>
       </c>
-      <c r="D83" s="8"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>30</v>
       </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8">
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5">
         <v>2300</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>31</v>
       </c>
-      <c r="B85" s="8">
+      <c r="B85" s="5">
         <v>23600</v>
       </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+      <c r="B87" s="17"/>
+      <c r="C87" s="17"/>
+      <c r="D87" s="18"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8">
+      <c r="B89" s="5"/>
+      <c r="C89" s="5">
         <v>20000</v>
       </c>
-      <c r="D89" s="8"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>29</v>
       </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8">
+      <c r="B90" s="5"/>
+      <c r="C90" s="5">
         <v>3600</v>
       </c>
-      <c r="D90" s="8"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>30</v>
       </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8">
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5">
         <v>18600</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>31</v>
       </c>
-      <c r="B92" s="8">
+      <c r="B92" s="5">
         <v>18600</v>
       </c>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>33</v>
       </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8">
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5">
         <v>5000</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="3"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+      <c r="B95" s="17"/>
+      <c r="C95" s="17"/>
+      <c r="D95" s="18"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="C96" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D96" s="6" t="s">
+      <c r="D96" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>28</v>
       </c>
-      <c r="B97" s="8"/>
-      <c r="C97" s="8">
+      <c r="B97" s="5"/>
+      <c r="C97" s="5">
         <v>20000</v>
       </c>
-      <c r="D97" s="8"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="5"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>29</v>
       </c>
-      <c r="B98" s="8"/>
-      <c r="C98" s="8">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5">
         <v>3600</v>
       </c>
-      <c r="D98" s="8"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>26</v>
       </c>
-      <c r="B99" s="8"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="8">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5">
         <v>23600</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="3"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+      <c r="B101" s="17"/>
+      <c r="C101" s="17"/>
+      <c r="D101" s="18"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C102" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="6" t="s">
+      <c r="D102" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>36</v>
       </c>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8">
+      <c r="B103" s="5"/>
+      <c r="C103" s="5">
         <v>300</v>
       </c>
-      <c r="D103" s="8"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>37</v>
       </c>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8">
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5">
         <v>300</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="3"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+      <c r="B106" s="17"/>
+      <c r="C106" s="17"/>
+      <c r="D106" s="18"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="6" t="s">
+      <c r="C107" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="6" t="s">
+      <c r="D107" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>39</v>
       </c>
-      <c r="B108" s="8"/>
-      <c r="C108" s="8">
+      <c r="B108" s="5"/>
+      <c r="C108" s="5">
         <v>2000</v>
       </c>
-      <c r="D108" s="8"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8">
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5">
         <v>2000</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="3"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="B111" s="17"/>
+      <c r="C111" s="17"/>
+      <c r="D111" s="18"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="C112" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D112" s="6" t="s">
+      <c r="D112" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>42</v>
       </c>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5">
         <v>15000</v>
       </c>
-      <c r="D113" s="8"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>40</v>
       </c>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5">
         <v>15000</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="3"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
+      <c r="B116" s="17"/>
+      <c r="C116" s="17"/>
+      <c r="D116" s="18"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C117" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D117" s="6" t="s">
+      <c r="D117" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>44</v>
       </c>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8">
+      <c r="B118" s="5"/>
+      <c r="C118" s="5">
         <v>30000</v>
       </c>
-      <c r="D118" s="8"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>45</v>
       </c>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5">
         <v>30000</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="3"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
+      <c r="B121" s="17"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="18"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C122" s="6" t="s">
+      <c r="C122" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D122" s="6" t="s">
+      <c r="D122" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>44</v>
       </c>
-      <c r="B123" s="8"/>
-      <c r="C123" s="8">
+      <c r="B123" s="5"/>
+      <c r="C123" s="5">
         <v>15000</v>
       </c>
-      <c r="D123" s="8"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>47</v>
       </c>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8">
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5">
         <v>15000</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="8"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="3"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
+      <c r="B126" s="17"/>
+      <c r="C126" s="17"/>
+      <c r="D126" s="18"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C127" s="6" t="s">
+      <c r="C127" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D127" s="6" t="s">
+      <c r="D127" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>40</v>
       </c>
-      <c r="B128" s="8"/>
-      <c r="C128" s="8">
+      <c r="B128" s="5"/>
+      <c r="C128" s="5">
         <v>25000</v>
       </c>
-      <c r="D128" s="8"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="5"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>49</v>
       </c>
-      <c r="B129" s="8"/>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8">
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5">
         <v>25000</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>50</v>
       </c>
-      <c r="B130" s="8">
+      <c r="B130" s="5">
         <v>25000</v>
       </c>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="3"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
+      <c r="B132" s="17"/>
+      <c r="C132" s="17"/>
+      <c r="D132" s="18"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C133" s="6" t="s">
+      <c r="C133" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D133" s="6" t="s">
+      <c r="D133" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>52</v>
       </c>
-      <c r="B134" s="8"/>
-      <c r="C134" s="8">
+      <c r="B134" s="5"/>
+      <c r="C134" s="5">
         <v>25000</v>
       </c>
-      <c r="D134" s="8"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D134" s="5"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>49</v>
       </c>
-      <c r="B135" s="8"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="8">
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5">
         <v>25000</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>50</v>
       </c>
-      <c r="B136" s="8">
+      <c r="B136" s="5">
         <v>25000</v>
       </c>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="8"/>
-      <c r="C137" s="8"/>
-      <c r="D137" s="8"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="3"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="4" t="s">
+      <c r="B138" s="17"/>
+      <c r="C138" s="17"/>
+      <c r="D138" s="18"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="B139" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C139" s="6" t="s">
+      <c r="C139" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D139" s="6" t="s">
+      <c r="D139" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>54</v>
       </c>
-      <c r="B140" s="8"/>
-      <c r="C140" s="8">
+      <c r="B140" s="5"/>
+      <c r="C140" s="5">
         <v>50000</v>
       </c>
-      <c r="D140" s="8"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D140" s="5"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>55</v>
       </c>
-      <c r="B141" s="8"/>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8">
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5">
         <v>50000</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="16"/>
-      <c r="B142" s="17"/>
-      <c r="C142" s="18"/>
-      <c r="D142" s="18"/>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="8"/>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="13"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="15"/>
+      <c r="D142" s="15"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="3"/>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="4" t="s">
+      <c r="B144" s="17"/>
+      <c r="C144" s="17"/>
+      <c r="D144" s="18"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B145" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C145" s="6" t="s">
+      <c r="C145" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D145" s="6" t="s">
+      <c r="D145" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>55</v>
       </c>
-      <c r="B146" s="8"/>
-      <c r="C146" s="8">
+      <c r="B146" s="5"/>
+      <c r="C146" s="5">
         <v>50000</v>
       </c>
-      <c r="D146" s="8"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>42</v>
       </c>
-      <c r="B147" s="8"/>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8">
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5">
         <v>48000</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>57</v>
       </c>
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8">
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5">
         <v>1200</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>58</v>
       </c>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8">
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5">
         <v>800</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="3"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="4" t="s">
+      <c r="B151" s="17"/>
+      <c r="C151" s="17"/>
+      <c r="D151" s="18"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C152" s="6" t="s">
+      <c r="C152" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D152" s="6" t="s">
+      <c r="D152" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>60</v>
       </c>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8">
+      <c r="B153" s="5"/>
+      <c r="C153" s="5">
         <v>5000</v>
       </c>
-      <c r="D153" s="8"/>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="5"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>45</v>
       </c>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8">
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5">
         <v>5000</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="3"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="4" t="s">
+      <c r="B156" s="17"/>
+      <c r="C156" s="17"/>
+      <c r="D156" s="18"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B157" s="5" t="s">
+      <c r="B157" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C157" s="6" t="s">
+      <c r="C157" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D157" s="6" t="s">
+      <c r="D157" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>62</v>
       </c>
-      <c r="B158" s="8"/>
-      <c r="C158" s="8">
+      <c r="B158" s="5"/>
+      <c r="C158" s="5">
         <v>15000</v>
       </c>
-      <c r="D158" s="8"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="5"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>63</v>
       </c>
-      <c r="B159" s="8"/>
-      <c r="C159" s="8">
+      <c r="B159" s="5"/>
+      <c r="C159" s="5">
         <v>2700</v>
       </c>
-      <c r="D159" s="8"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="5"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>45</v>
       </c>
-      <c r="B160" s="8"/>
-      <c r="C160" s="8"/>
-      <c r="D160" s="8">
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5">
         <v>13500</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>64</v>
       </c>
-      <c r="B161" s="8"/>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8">
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5">
         <v>1500</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>65</v>
       </c>
-      <c r="B162" s="8"/>
-      <c r="C162" s="8"/>
-      <c r="D162" s="8">
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5">
         <v>2700</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="8"/>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="3"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
+      <c r="B164" s="17"/>
+      <c r="C164" s="17"/>
+      <c r="D164" s="18"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B165" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C165" s="6" t="s">
+      <c r="C165" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D165" s="6" t="s">
+      <c r="D165" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>64</v>
       </c>
-      <c r="B166" s="8"/>
-      <c r="C166" s="8">
+      <c r="B166" s="5"/>
+      <c r="C166" s="5">
         <v>1500</v>
       </c>
-      <c r="D166" s="8"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D166" s="5"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>42</v>
       </c>
-      <c r="B167" s="8"/>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8">
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5">
         <v>1500</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="8"/>
-      <c r="C168" s="8"/>
-      <c r="D168" s="8"/>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-      <c r="D169" s="3"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="4" t="s">
+      <c r="B169" s="17"/>
+      <c r="C169" s="17"/>
+      <c r="D169" s="18"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B170" s="5" t="s">
+      <c r="B170" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C170" s="6" t="s">
+      <c r="C170" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D170" s="6" t="s">
+      <c r="D170" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>65</v>
       </c>
-      <c r="B171" s="8"/>
-      <c r="C171" s="8">
+      <c r="B171" s="5"/>
+      <c r="C171" s="5">
         <v>2700</v>
       </c>
-      <c r="D171" s="8"/>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D171" s="5"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>42</v>
       </c>
-      <c r="B172" s="8"/>
-      <c r="C172" s="8"/>
-      <c r="D172" s="8">
+      <c r="B172" s="5"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5">
         <v>2700</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A138:D138"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="A151:D151"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A164:D164"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A95:D95"/>
     <mergeCell ref="A169:D169"/>
     <mergeCell ref="A106:D106"/>
     <mergeCell ref="A111:D111"/>
@@ -2329,18 +2357,11 @@
     <mergeCell ref="A121:D121"/>
     <mergeCell ref="A126:D126"/>
     <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A138:D138"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="A151:D151"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A164:D164"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>